<commit_message>
Atualização de bases das ligas, do dia: 24-02-2024 às 13:41
</commit_message>
<xml_diff>
--- a/Uruguay Primera División/Uruguay Primera División.xlsx
+++ b/Uruguay Primera División/Uruguay Primera División.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="52">
   <si>
     <t>id</t>
   </si>
@@ -531,7 +531,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC247"/>
+  <dimension ref="A1:AC253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -21187,7 +21187,7 @@
         <v>231</v>
       </c>
       <c r="B233">
-        <v>7559469</v>
+        <v>7559468</v>
       </c>
       <c r="C233" t="s">
         <v>28</v>
@@ -21199,76 +21199,76 @@
         <v>45266.70833333334</v>
       </c>
       <c r="F233" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G233" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="H233">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I233">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J233" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K233">
-        <v>4.75</v>
+        <v>1.7</v>
       </c>
       <c r="L233">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="M233">
-        <v>1.7</v>
+        <v>5.75</v>
       </c>
       <c r="N233">
-        <v>2.7</v>
+        <v>1.833</v>
       </c>
       <c r="O233">
         <v>3.2</v>
       </c>
       <c r="P233">
-        <v>2.45</v>
+        <v>4.5</v>
       </c>
       <c r="Q233">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R233">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="S233">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="T233">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="U233">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="V233">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="W233">
-        <v>-1</v>
+        <v>0.833</v>
       </c>
       <c r="X233">
-        <v>2.2</v>
+        <v>-1</v>
       </c>
       <c r="Y233">
         <v>-1</v>
       </c>
       <c r="Z233">
-        <v>0</v>
+        <v>0.925</v>
       </c>
       <c r="AA233">
-        <v>-0</v>
+        <v>-1</v>
       </c>
       <c r="AB233">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AC233">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="234" spans="1:29">
@@ -21276,7 +21276,7 @@
         <v>232</v>
       </c>
       <c r="B234">
-        <v>7559468</v>
+        <v>7559469</v>
       </c>
       <c r="C234" t="s">
         <v>28</v>
@@ -21288,76 +21288,76 @@
         <v>45266.70833333334</v>
       </c>
       <c r="F234" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G234" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="H234">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I234">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J234" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K234">
+        <v>4.75</v>
+      </c>
+      <c r="L234">
+        <v>3.4</v>
+      </c>
+      <c r="M234">
         <v>1.7</v>
       </c>
-      <c r="L234">
-        <v>3</v>
-      </c>
-      <c r="M234">
-        <v>5.75</v>
-      </c>
       <c r="N234">
-        <v>1.833</v>
+        <v>2.7</v>
       </c>
       <c r="O234">
         <v>3.2</v>
       </c>
       <c r="P234">
-        <v>4.5</v>
+        <v>2.45</v>
       </c>
       <c r="Q234">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="R234">
-        <v>1.925</v>
+        <v>2.05</v>
       </c>
       <c r="S234">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="T234">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="U234">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="V234">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="W234">
-        <v>0.833</v>
+        <v>-1</v>
       </c>
       <c r="X234">
-        <v>-1</v>
+        <v>2.2</v>
       </c>
       <c r="Y234">
         <v>-1</v>
       </c>
       <c r="Z234">
-        <v>0.925</v>
+        <v>0</v>
       </c>
       <c r="AA234">
-        <v>-1</v>
+        <v>-0</v>
       </c>
       <c r="AB234">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AC234">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="235" spans="1:29">
@@ -21454,7 +21454,7 @@
         <v>234</v>
       </c>
       <c r="B236">
-        <v>7013885</v>
+        <v>7013409</v>
       </c>
       <c r="C236" t="s">
         <v>28</v>
@@ -21466,76 +21466,76 @@
         <v>45267.70833333334</v>
       </c>
       <c r="F236" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G236" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H236">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I236">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J236" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K236">
+        <v>1.666</v>
+      </c>
+      <c r="L236">
+        <v>3.9</v>
+      </c>
+      <c r="M236">
+        <v>4.5</v>
+      </c>
+      <c r="N236">
+        <v>1.615</v>
+      </c>
+      <c r="O236">
+        <v>4</v>
+      </c>
+      <c r="P236">
+        <v>4.75</v>
+      </c>
+      <c r="Q236">
+        <v>-0.75</v>
+      </c>
+      <c r="R236">
+        <v>1.8</v>
+      </c>
+      <c r="S236">
+        <v>2.05</v>
+      </c>
+      <c r="T236">
+        <v>2.75</v>
+      </c>
+      <c r="U236">
+        <v>1.95</v>
+      </c>
+      <c r="V236">
+        <v>1.9</v>
+      </c>
+      <c r="W236">
+        <v>-1</v>
+      </c>
+      <c r="X236">
         <v>3</v>
       </c>
-      <c r="L236">
-        <v>3</v>
-      </c>
-      <c r="M236">
-        <v>2.4</v>
-      </c>
-      <c r="N236">
-        <v>2.9</v>
-      </c>
-      <c r="O236">
-        <v>2.75</v>
-      </c>
-      <c r="P236">
-        <v>2.6</v>
-      </c>
-      <c r="Q236">
-        <v>0</v>
-      </c>
-      <c r="R236">
-        <v>2.025</v>
-      </c>
-      <c r="S236">
-        <v>1.825</v>
-      </c>
-      <c r="T236">
-        <v>2</v>
-      </c>
-      <c r="U236">
-        <v>2.025</v>
-      </c>
-      <c r="V236">
-        <v>1.825</v>
-      </c>
-      <c r="W236">
-        <v>-1</v>
-      </c>
-      <c r="X236">
-        <v>-1</v>
-      </c>
       <c r="Y236">
-        <v>1.6</v>
+        <v>-1</v>
       </c>
       <c r="Z236">
         <v>-1</v>
       </c>
       <c r="AA236">
-        <v>0.825</v>
+        <v>1.05</v>
       </c>
       <c r="AB236">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC236">
-        <v>-0</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="237" spans="1:29">
@@ -21632,7 +21632,7 @@
         <v>236</v>
       </c>
       <c r="B238">
-        <v>7013409</v>
+        <v>7013886</v>
       </c>
       <c r="C238" t="s">
         <v>28</v>
@@ -21644,76 +21644,76 @@
         <v>45267.70833333334</v>
       </c>
       <c r="F238" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G238" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="H238">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I238">
         <v>1</v>
       </c>
       <c r="J238" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K238">
-        <v>1.666</v>
+        <v>2.25</v>
       </c>
       <c r="L238">
-        <v>3.9</v>
+        <v>3.1</v>
       </c>
       <c r="M238">
-        <v>4.5</v>
+        <v>3.25</v>
       </c>
       <c r="N238">
-        <v>1.615</v>
+        <v>2.25</v>
       </c>
       <c r="O238">
-        <v>4</v>
+        <v>2.875</v>
       </c>
       <c r="P238">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="Q238">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="R238">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="S238">
-        <v>2.05</v>
+        <v>1.9</v>
       </c>
       <c r="T238">
-        <v>2.75</v>
+        <v>2</v>
       </c>
       <c r="U238">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V238">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W238">
         <v>-1</v>
       </c>
       <c r="X238">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Y238">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Z238">
         <v>-1</v>
       </c>
       <c r="AA238">
-        <v>1.05</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB238">
         <v>-1</v>
       </c>
       <c r="AC238">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="239" spans="1:29">
@@ -21721,7 +21721,7 @@
         <v>237</v>
       </c>
       <c r="B239">
-        <v>7013886</v>
+        <v>7013885</v>
       </c>
       <c r="C239" t="s">
         <v>28</v>
@@ -21733,55 +21733,55 @@
         <v>45267.70833333334</v>
       </c>
       <c r="F239" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G239" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H239">
         <v>0</v>
       </c>
       <c r="I239">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J239" t="s">
         <v>49</v>
       </c>
       <c r="K239">
-        <v>2.25</v>
+        <v>3</v>
       </c>
       <c r="L239">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="M239">
-        <v>3.25</v>
+        <v>2.4</v>
       </c>
       <c r="N239">
-        <v>2.25</v>
+        <v>2.9</v>
       </c>
       <c r="O239">
-        <v>2.875</v>
+        <v>2.75</v>
       </c>
       <c r="P239">
-        <v>3.5</v>
+        <v>2.6</v>
       </c>
       <c r="Q239">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R239">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="S239">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="T239">
         <v>2</v>
       </c>
       <c r="U239">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="V239">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="W239">
         <v>-1</v>
@@ -21790,19 +21790,19 @@
         <v>-1</v>
       </c>
       <c r="Y239">
-        <v>2.5</v>
+        <v>1.6</v>
       </c>
       <c r="Z239">
         <v>-1</v>
       </c>
       <c r="AA239">
-        <v>0.8999999999999999</v>
+        <v>0.825</v>
       </c>
       <c r="AB239">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC239">
-        <v>0.925</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="240" spans="1:29">
@@ -21894,7 +21894,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="241" spans="1:27">
+    <row r="241" spans="1:29">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -21916,6 +21916,15 @@
       <c r="G241" t="s">
         <v>40</v>
       </c>
+      <c r="H241">
+        <v>2</v>
+      </c>
+      <c r="I241">
+        <v>1</v>
+      </c>
+      <c r="J241" t="s">
+        <v>50</v>
+      </c>
       <c r="K241">
         <v>1.6</v>
       </c>
@@ -21953,22 +21962,28 @@
         <v>2.025</v>
       </c>
       <c r="W241">
-        <v>0</v>
+        <v>0.55</v>
       </c>
       <c r="X241">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y241">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z241">
         <v>0</v>
       </c>
       <c r="AA241">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="242" spans="1:27">
+        <v>-0</v>
+      </c>
+      <c r="AB241">
+        <v>0.825</v>
+      </c>
+      <c r="AC241">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:29">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -21990,6 +22005,15 @@
       <c r="G242" t="s">
         <v>43</v>
       </c>
+      <c r="H242">
+        <v>1</v>
+      </c>
+      <c r="I242">
+        <v>2</v>
+      </c>
+      <c r="J242" t="s">
+        <v>49</v>
+      </c>
       <c r="K242">
         <v>2.6</v>
       </c>
@@ -22000,49 +22024,55 @@
         <v>2.9</v>
       </c>
       <c r="N242">
+        <v>2.75</v>
+      </c>
+      <c r="O242">
         <v>2.875</v>
       </c>
-      <c r="O242">
-        <v>2.9</v>
-      </c>
       <c r="P242">
-        <v>2.625</v>
+        <v>2.75</v>
       </c>
       <c r="Q242">
         <v>0</v>
       </c>
       <c r="R242">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="S242">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="T242">
         <v>2</v>
       </c>
       <c r="U242">
-        <v>2.025</v>
+        <v>2.1</v>
       </c>
       <c r="V242">
-        <v>1.825</v>
+        <v>1.775</v>
       </c>
       <c r="W242">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X242">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y242">
-        <v>0</v>
+        <v>1.75</v>
       </c>
       <c r="Z242">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA242">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="243" spans="1:27">
+        <v>0.95</v>
+      </c>
+      <c r="AB242">
+        <v>1.1</v>
+      </c>
+      <c r="AC242">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:29">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -22064,6 +22094,15 @@
       <c r="G243" t="s">
         <v>48</v>
       </c>
+      <c r="H243">
+        <v>2</v>
+      </c>
+      <c r="I243">
+        <v>3</v>
+      </c>
+      <c r="J243" t="s">
+        <v>49</v>
+      </c>
       <c r="K243">
         <v>2.5</v>
       </c>
@@ -22074,49 +22113,55 @@
         <v>2.8</v>
       </c>
       <c r="N243">
-        <v>2.45</v>
+        <v>2.4</v>
       </c>
       <c r="O243">
         <v>3.2</v>
       </c>
       <c r="P243">
-        <v>2.875</v>
+        <v>2.9</v>
       </c>
       <c r="Q243">
         <v>0</v>
       </c>
       <c r="R243">
-        <v>1.75</v>
+        <v>1.725</v>
       </c>
       <c r="S243">
-        <v>2.125</v>
+        <v>2.075</v>
       </c>
       <c r="T243">
         <v>2</v>
       </c>
       <c r="U243">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="V243">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="W243">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X243">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y243">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="Z243">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA243">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="244" spans="1:27">
+        <v>1.075</v>
+      </c>
+      <c r="AB243">
+        <v>0.825</v>
+      </c>
+      <c r="AC243">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:29">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -22138,6 +22183,15 @@
       <c r="G244" t="s">
         <v>42</v>
       </c>
+      <c r="H244">
+        <v>1</v>
+      </c>
+      <c r="I244">
+        <v>2</v>
+      </c>
+      <c r="J244" t="s">
+        <v>49</v>
+      </c>
       <c r="K244">
         <v>2.3</v>
       </c>
@@ -22154,7 +22208,7 @@
         <v>3.2</v>
       </c>
       <c r="P244">
-        <v>3.2</v>
+        <v>3.25</v>
       </c>
       <c r="Q244">
         <v>-0.25</v>
@@ -22169,28 +22223,34 @@
         <v>2.25</v>
       </c>
       <c r="U244">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="V244">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W244">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X244">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y244">
-        <v>0</v>
+        <v>2.25</v>
       </c>
       <c r="Z244">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA244">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="245" spans="1:27">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="AB244">
+        <v>0.95</v>
+      </c>
+      <c r="AC244">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:29">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -22212,6 +22272,15 @@
       <c r="G245" t="s">
         <v>44</v>
       </c>
+      <c r="H245">
+        <v>1</v>
+      </c>
+      <c r="I245">
+        <v>1</v>
+      </c>
+      <c r="J245" t="s">
+        <v>51</v>
+      </c>
       <c r="K245">
         <v>2.4</v>
       </c>
@@ -22222,49 +22291,55 @@
         <v>3.25</v>
       </c>
       <c r="N245">
-        <v>2.55</v>
+        <v>2.625</v>
       </c>
       <c r="O245">
         <v>3</v>
       </c>
       <c r="P245">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="Q245">
         <v>0</v>
       </c>
       <c r="R245">
-        <v>1.75</v>
+        <v>1.775</v>
       </c>
       <c r="S245">
-        <v>2.125</v>
+        <v>2.1</v>
       </c>
       <c r="T245">
         <v>2</v>
       </c>
       <c r="U245">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="V245">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="W245">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X245">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y245">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z245">
         <v>0</v>
       </c>
       <c r="AA245">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="246" spans="1:27">
+        <v>-0</v>
+      </c>
+      <c r="AB245">
+        <v>0</v>
+      </c>
+      <c r="AC245">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:29">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -22286,6 +22361,15 @@
       <c r="G246" t="s">
         <v>46</v>
       </c>
+      <c r="H246">
+        <v>2</v>
+      </c>
+      <c r="I246">
+        <v>2</v>
+      </c>
+      <c r="J246" t="s">
+        <v>51</v>
+      </c>
       <c r="K246">
         <v>3.8</v>
       </c>
@@ -22296,49 +22380,55 @@
         <v>1.95</v>
       </c>
       <c r="N246">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="O246">
-        <v>3.25</v>
+        <v>3.2</v>
       </c>
       <c r="P246">
-        <v>2.1</v>
+        <v>2.4</v>
       </c>
       <c r="Q246">
         <v>0.25</v>
       </c>
       <c r="R246">
-        <v>2.05</v>
+        <v>1.775</v>
       </c>
       <c r="S246">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="T246">
         <v>2.25</v>
       </c>
       <c r="U246">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="V246">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="W246">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X246">
-        <v>0</v>
+        <v>2.2</v>
       </c>
       <c r="Y246">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z246">
-        <v>0</v>
+        <v>0.3875</v>
       </c>
       <c r="AA246">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="247" spans="1:27">
+        <v>-0.5</v>
+      </c>
+      <c r="AB246">
+        <v>1.025</v>
+      </c>
+      <c r="AC246">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:29">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -22360,6 +22450,15 @@
       <c r="G247" t="s">
         <v>32</v>
       </c>
+      <c r="H247">
+        <v>1</v>
+      </c>
+      <c r="I247">
+        <v>2</v>
+      </c>
+      <c r="J247" t="s">
+        <v>49</v>
+      </c>
       <c r="K247">
         <v>5.25</v>
       </c>
@@ -22370,10 +22469,10 @@
         <v>1.7</v>
       </c>
       <c r="N247">
-        <v>5.5</v>
+        <v>5.75</v>
       </c>
       <c r="O247">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="P247">
         <v>1.666</v>
@@ -22382,33 +22481,498 @@
         <v>0.75</v>
       </c>
       <c r="R247">
+        <v>1.9</v>
+      </c>
+      <c r="S247">
+        <v>1.95</v>
+      </c>
+      <c r="T247">
+        <v>2</v>
+      </c>
+      <c r="U247">
+        <v>1.95</v>
+      </c>
+      <c r="V247">
+        <v>1.9</v>
+      </c>
+      <c r="W247">
+        <v>-1</v>
+      </c>
+      <c r="X247">
+        <v>-1</v>
+      </c>
+      <c r="Y247">
+        <v>0.6659999999999999</v>
+      </c>
+      <c r="Z247">
+        <v>-0.5</v>
+      </c>
+      <c r="AA247">
+        <v>0.475</v>
+      </c>
+      <c r="AB247">
+        <v>0.95</v>
+      </c>
+      <c r="AC247">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:29">
+      <c r="A248" s="1">
+        <v>246</v>
+      </c>
+      <c r="B248">
+        <v>7825144</v>
+      </c>
+      <c r="C248" t="s">
+        <v>28</v>
+      </c>
+      <c r="D248" t="s">
+        <v>29</v>
+      </c>
+      <c r="E248" s="2">
+        <v>45345.70833333334</v>
+      </c>
+      <c r="F248" t="s">
+        <v>40</v>
+      </c>
+      <c r="G248" t="s">
+        <v>41</v>
+      </c>
+      <c r="H248">
+        <v>3</v>
+      </c>
+      <c r="I248">
+        <v>1</v>
+      </c>
+      <c r="J248" t="s">
+        <v>50</v>
+      </c>
+      <c r="K248">
+        <v>2.375</v>
+      </c>
+      <c r="L248">
+        <v>3.1</v>
+      </c>
+      <c r="M248">
+        <v>3</v>
+      </c>
+      <c r="N248">
+        <v>2.375</v>
+      </c>
+      <c r="O248">
+        <v>3.1</v>
+      </c>
+      <c r="P248">
+        <v>3</v>
+      </c>
+      <c r="Q248">
+        <v>-0.25</v>
+      </c>
+      <c r="R248">
+        <v>2.05</v>
+      </c>
+      <c r="S248">
+        <v>1.8</v>
+      </c>
+      <c r="T248">
+        <v>2.25</v>
+      </c>
+      <c r="U248">
+        <v>2.025</v>
+      </c>
+      <c r="V248">
+        <v>1.825</v>
+      </c>
+      <c r="W248">
+        <v>1.375</v>
+      </c>
+      <c r="X248">
+        <v>-1</v>
+      </c>
+      <c r="Y248">
+        <v>-1</v>
+      </c>
+      <c r="Z248">
+        <v>1.05</v>
+      </c>
+      <c r="AA248">
+        <v>-1</v>
+      </c>
+      <c r="AB248">
+        <v>1.025</v>
+      </c>
+      <c r="AC248">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:29">
+      <c r="A249" s="1">
+        <v>247</v>
+      </c>
+      <c r="B249">
+        <v>7825143</v>
+      </c>
+      <c r="C249" t="s">
+        <v>28</v>
+      </c>
+      <c r="D249" t="s">
+        <v>29</v>
+      </c>
+      <c r="E249" s="2">
+        <v>45346.70833333334</v>
+      </c>
+      <c r="F249" t="s">
+        <v>42</v>
+      </c>
+      <c r="G249" t="s">
+        <v>43</v>
+      </c>
+      <c r="K249">
+        <v>2.75</v>
+      </c>
+      <c r="L249">
+        <v>3.1</v>
+      </c>
+      <c r="M249">
+        <v>2.5</v>
+      </c>
+      <c r="N249">
+        <v>2.55</v>
+      </c>
+      <c r="O249">
+        <v>3.1</v>
+      </c>
+      <c r="P249">
+        <v>2.7</v>
+      </c>
+      <c r="Q249">
+        <v>0</v>
+      </c>
+      <c r="R249">
+        <v>1.875</v>
+      </c>
+      <c r="S249">
+        <v>1.975</v>
+      </c>
+      <c r="T249">
+        <v>2.25</v>
+      </c>
+      <c r="U249">
+        <v>1.95</v>
+      </c>
+      <c r="V249">
+        <v>1.9</v>
+      </c>
+      <c r="W249">
+        <v>0</v>
+      </c>
+      <c r="X249">
+        <v>0</v>
+      </c>
+      <c r="Y249">
+        <v>0</v>
+      </c>
+      <c r="Z249">
+        <v>0</v>
+      </c>
+      <c r="AA249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:29">
+      <c r="A250" s="1">
+        <v>248</v>
+      </c>
+      <c r="B250">
+        <v>7825103</v>
+      </c>
+      <c r="C250" t="s">
+        <v>28</v>
+      </c>
+      <c r="D250" t="s">
+        <v>29</v>
+      </c>
+      <c r="E250" s="2">
+        <v>45346.83333333334</v>
+      </c>
+      <c r="F250" t="s">
+        <v>32</v>
+      </c>
+      <c r="G250" t="s">
+        <v>47</v>
+      </c>
+      <c r="K250">
+        <v>1.4</v>
+      </c>
+      <c r="L250">
+        <v>4</v>
+      </c>
+      <c r="M250">
+        <v>9</v>
+      </c>
+      <c r="N250">
+        <v>1.363</v>
+      </c>
+      <c r="O250">
+        <v>4.333</v>
+      </c>
+      <c r="P250">
+        <v>9</v>
+      </c>
+      <c r="Q250">
+        <v>-1.25</v>
+      </c>
+      <c r="R250">
+        <v>1.875</v>
+      </c>
+      <c r="S250">
+        <v>1.975</v>
+      </c>
+      <c r="T250">
+        <v>2.5</v>
+      </c>
+      <c r="U250">
+        <v>1.975</v>
+      </c>
+      <c r="V250">
+        <v>1.875</v>
+      </c>
+      <c r="W250">
+        <v>0</v>
+      </c>
+      <c r="X250">
+        <v>0</v>
+      </c>
+      <c r="Y250">
+        <v>0</v>
+      </c>
+      <c r="Z250">
+        <v>0</v>
+      </c>
+      <c r="AA250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:29">
+      <c r="A251" s="1">
+        <v>249</v>
+      </c>
+      <c r="B251">
+        <v>7825146</v>
+      </c>
+      <c r="C251" t="s">
+        <v>28</v>
+      </c>
+      <c r="D251" t="s">
+        <v>29</v>
+      </c>
+      <c r="E251" s="2">
+        <v>45347.41666666666</v>
+      </c>
+      <c r="F251" t="s">
+        <v>33</v>
+      </c>
+      <c r="G251" t="s">
+        <v>39</v>
+      </c>
+      <c r="K251">
+        <v>2.625</v>
+      </c>
+      <c r="L251">
+        <v>2.875</v>
+      </c>
+      <c r="M251">
+        <v>2.75</v>
+      </c>
+      <c r="N251">
+        <v>2.45</v>
+      </c>
+      <c r="O251">
+        <v>2.875</v>
+      </c>
+      <c r="P251">
+        <v>3</v>
+      </c>
+      <c r="Q251">
+        <v>-0.25</v>
+      </c>
+      <c r="R251">
+        <v>2.125</v>
+      </c>
+      <c r="S251">
+        <v>1.75</v>
+      </c>
+      <c r="T251">
+        <v>2</v>
+      </c>
+      <c r="U251">
+        <v>1.975</v>
+      </c>
+      <c r="V251">
+        <v>1.875</v>
+      </c>
+      <c r="W251">
+        <v>0</v>
+      </c>
+      <c r="X251">
+        <v>0</v>
+      </c>
+      <c r="Y251">
+        <v>0</v>
+      </c>
+      <c r="Z251">
+        <v>0</v>
+      </c>
+      <c r="AA251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:29">
+      <c r="A252" s="1">
+        <v>250</v>
+      </c>
+      <c r="B252">
+        <v>7825104</v>
+      </c>
+      <c r="C252" t="s">
+        <v>28</v>
+      </c>
+      <c r="D252" t="s">
+        <v>29</v>
+      </c>
+      <c r="E252" s="2">
+        <v>45347.70833333334</v>
+      </c>
+      <c r="F252" t="s">
+        <v>46</v>
+      </c>
+      <c r="G252" t="s">
+        <v>36</v>
+      </c>
+      <c r="K252">
+        <v>2.875</v>
+      </c>
+      <c r="L252">
+        <v>3.3</v>
+      </c>
+      <c r="M252">
+        <v>2.375</v>
+      </c>
+      <c r="N252">
+        <v>2.75</v>
+      </c>
+      <c r="O252">
+        <v>3.3</v>
+      </c>
+      <c r="P252">
+        <v>2.45</v>
+      </c>
+      <c r="Q252">
+        <v>0</v>
+      </c>
+      <c r="R252">
+        <v>2.05</v>
+      </c>
+      <c r="S252">
+        <v>1.8</v>
+      </c>
+      <c r="T252">
+        <v>2.5</v>
+      </c>
+      <c r="U252">
         <v>1.925</v>
       </c>
-      <c r="S247">
+      <c r="V252">
         <v>1.925</v>
       </c>
-      <c r="T247">
-        <v>2</v>
-      </c>
-      <c r="U247">
-        <v>1.85</v>
-      </c>
-      <c r="V247">
-        <v>2</v>
-      </c>
-      <c r="W247">
-        <v>0</v>
-      </c>
-      <c r="X247">
-        <v>0</v>
-      </c>
-      <c r="Y247">
-        <v>0</v>
-      </c>
-      <c r="Z247">
-        <v>0</v>
-      </c>
-      <c r="AA247">
+      <c r="W252">
+        <v>0</v>
+      </c>
+      <c r="X252">
+        <v>0</v>
+      </c>
+      <c r="Y252">
+        <v>0</v>
+      </c>
+      <c r="Z252">
+        <v>0</v>
+      </c>
+      <c r="AA252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:29">
+      <c r="A253" s="1">
+        <v>251</v>
+      </c>
+      <c r="B253">
+        <v>7825147</v>
+      </c>
+      <c r="C253" t="s">
+        <v>28</v>
+      </c>
+      <c r="D253" t="s">
+        <v>29</v>
+      </c>
+      <c r="E253" s="2">
+        <v>45347.8125</v>
+      </c>
+      <c r="F253" t="s">
+        <v>38</v>
+      </c>
+      <c r="G253" t="s">
+        <v>45</v>
+      </c>
+      <c r="K253">
+        <v>1.727</v>
+      </c>
+      <c r="L253">
+        <v>3.6</v>
+      </c>
+      <c r="M253">
+        <v>4.333</v>
+      </c>
+      <c r="N253">
+        <v>1.7</v>
+      </c>
+      <c r="O253">
+        <v>3.6</v>
+      </c>
+      <c r="P253">
+        <v>4.5</v>
+      </c>
+      <c r="Q253">
+        <v>-0.75</v>
+      </c>
+      <c r="R253">
+        <v>1.975</v>
+      </c>
+      <c r="S253">
+        <v>1.875</v>
+      </c>
+      <c r="T253">
+        <v>2.5</v>
+      </c>
+      <c r="U253">
+        <v>2.05</v>
+      </c>
+      <c r="V253">
+        <v>1.8</v>
+      </c>
+      <c r="W253">
+        <v>0</v>
+      </c>
+      <c r="X253">
+        <v>0</v>
+      </c>
+      <c r="Y253">
+        <v>0</v>
+      </c>
+      <c r="Z253">
+        <v>0</v>
+      </c>
+      <c r="AA253">
         <v>0</v>
       </c>
     </row>

</xml_diff>